<commit_message>
Improved the example case and added template images for general and product-specific use.
</commit_message>
<xml_diff>
--- a/example_excel/Product list example.xlsx
+++ b/example_excel/Product list example.xlsx
@@ -1110,7 +1110,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3251,7 +3251,7 @@
   <customSheetViews>
     <customSheetView guid="{E30E9127-79F7-452D-AB9E-91F6C97BF535}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="C1:Q706" xr:uid="{0492C9B2-70F8-415E-9E83-EC18560F2CF6}"/>
+      <autoFilter ref="C1:Q706" xr:uid="{685837C6-7B73-4552-8393-D88ABACC57CE}"/>
     </customSheetView>
   </customSheetViews>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>